<commit_message>
upgrade data of year 2020
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adyliu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adyliu/codes/github/china_area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A3BBD00-B25D-104C-89EE-84057874160B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A0865E-6C90-FA42-9B1D-96BB6493E676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16240" xr2:uid="{5888D5A7-D7A2-FC4B-8093-B0573B8EE50E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>级别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +66,10 @@
   </si>
   <si>
     <t>同比去年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -67,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +119,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -126,24 +153,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -459,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8280C78-A2C3-D342-A566-BA79FC172DBC}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -473,218 +533,300 @@
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="26">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3">
         <v>2019</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="3"/>
+      <c r="G1" s="3">
+        <v>2018</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="4">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="31">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="E2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1">
-        <v>2017</v>
-      </c>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" ht="31">
-      <c r="A2" s="2">
+      <c r="G2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="31">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C3" s="6">
         <v>31</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
         <v>31</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
         <v>31</v>
       </c>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="31">
-      <c r="A3" s="2">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="31">
+      <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C4" s="6">
+        <v>342</v>
+      </c>
+      <c r="D4" s="6">
+        <f>C4-E4</f>
+        <v>-1</v>
+      </c>
+      <c r="E4" s="6">
         <v>343</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
         <v>343</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6">
         <v>344</v>
       </c>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="31">
-      <c r="A4" s="2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="31">
+      <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="6">
+        <v>3272</v>
+      </c>
+      <c r="D5" s="6">
+        <f t="shared" ref="D5:D8" si="0">C5-E5</f>
+        <v>-10</v>
+      </c>
+      <c r="E5" s="6">
         <v>3282</v>
       </c>
-      <c r="D4" s="2">
-        <f>C4-E4</f>
+      <c r="F5" s="6">
+        <f>E5-G5</f>
         <v>-5</v>
       </c>
-      <c r="E4" s="2">
+      <c r="G5" s="6">
         <v>3287</v>
       </c>
-      <c r="F4" s="2">
-        <f>E4-G4</f>
+      <c r="H5" s="6">
+        <f>G5-I5</f>
         <v>154</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I5" s="6">
         <v>3133</v>
       </c>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="31">
-      <c r="A5" s="2">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="31">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="6">
+        <v>43104</v>
+      </c>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>-459</v>
+      </c>
+      <c r="E6" s="6">
         <v>43563</v>
       </c>
-      <c r="D5" s="2">
-        <f t="shared" ref="D5:D7" si="0">C5-E5</f>
+      <c r="F6" s="6">
+        <f t="shared" ref="F6:F8" si="1">E6-G6</f>
         <v>40</v>
       </c>
-      <c r="E5" s="2">
+      <c r="G6" s="6">
         <v>43523</v>
       </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F7" si="1">E5-G5</f>
+      <c r="H6" s="6">
+        <f t="shared" ref="H6:H8" si="2">G6-I6</f>
         <v>655</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I6" s="6">
         <v>42868</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="31">
-      <c r="A6" s="2">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="31">
+      <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="6">
+        <v>658001</v>
+      </c>
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>-8259</v>
+      </c>
+      <c r="E7" s="6">
         <v>666260</v>
       </c>
-      <c r="D6" s="2">
+      <c r="F7" s="6">
+        <f t="shared" si="1"/>
+        <v>-7478</v>
+      </c>
+      <c r="G7" s="6">
+        <v>673738</v>
+      </c>
+      <c r="H7" s="6">
+        <f t="shared" si="2"/>
+        <v>7083</v>
+      </c>
+      <c r="I7" s="6">
+        <v>666655</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="31">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="8">
+        <f>SUM(C3:C7)</f>
+        <v>704750</v>
+      </c>
+      <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>-7478</v>
-      </c>
-      <c r="E6" s="2">
-        <v>673738</v>
-      </c>
-      <c r="F6" s="2">
+        <v>-8729</v>
+      </c>
+      <c r="E8" s="7">
+        <f>SUM(E3:E7)</f>
+        <v>713479</v>
+      </c>
+      <c r="F8" s="7">
         <f t="shared" si="1"/>
-        <v>7083</v>
-      </c>
-      <c r="G6" s="2">
-        <v>666655</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="31">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3">
-        <f>SUM(C2:C6)</f>
-        <v>713479</v>
-      </c>
-      <c r="D7" s="3">
-        <f t="shared" si="0"/>
         <v>-7443</v>
       </c>
-      <c r="E7" s="3">
-        <f>SUM(E2:E6)</f>
+      <c r="G8" s="7">
+        <f>SUM(G3:G7)</f>
         <v>720922</v>
       </c>
-      <c r="F7" s="3">
-        <f t="shared" si="1"/>
+      <c r="H8" s="7">
+        <f t="shared" si="2"/>
         <v>7891</v>
       </c>
-      <c r="G7" s="3">
-        <f>SUM(G2:G6)</f>
+      <c r="I8" s="7">
+        <f>SUM(I3:I7)</f>
         <v>713031</v>
       </c>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="31">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="31">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="31">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="31">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="31">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="31">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="31">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" ht="31">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update data to 2021.10.31
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adyliu/codes/github/china_area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A0865E-6C90-FA42-9B1D-96BB6493E676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5C801B-7FBF-E641-95B8-469A0F8CD731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16240" xr2:uid="{5888D5A7-D7A2-FC4B-8093-B0573B8EE50E}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15940" xr2:uid="{5888D5A7-D7A2-FC4B-8093-B0573B8EE50E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>级别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,7 +77,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -136,6 +136,15 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FFC00000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -145,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -168,42 +177,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8280C78-A2C3-D342-A566-BA79FC172DBC}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -535,243 +582,344 @@
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" ht="26">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C1" s="12">
+        <v>2022</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="11">
+        <v>2021</v>
+      </c>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11">
         <v>2020</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11">
         <v>2019</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3">
+      <c r="J1" s="11"/>
+      <c r="K1" s="11">
         <v>2018</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="4">
+      <c r="L1" s="11"/>
+      <c r="M1" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="31">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="5" t="s">
+    <row r="2" spans="1:14" ht="31">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="31">
-      <c r="A3" s="6">
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="31">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>31</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4">
         <v>31</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
+      <c r="F3" s="4"/>
+      <c r="G3" s="4">
         <v>31</v>
       </c>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4">
         <v>31</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="31">
-      <c r="A4" s="6">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4">
+        <v>31</v>
+      </c>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="31">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="4">
+        <v>316</v>
+      </c>
+      <c r="D4" s="4">
+        <f>C4-E4</f>
+        <v>-26</v>
+      </c>
+      <c r="E4" s="4">
         <v>342</v>
       </c>
-      <c r="D4" s="6">
-        <f>C4-E4</f>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4">
+        <v>342</v>
+      </c>
+      <c r="H4" s="4">
+        <f>G4-I4</f>
         <v>-1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="I4" s="4">
         <v>343</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4">
         <v>343</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6">
+      <c r="L4" s="4"/>
+      <c r="M4" s="4">
         <v>344</v>
       </c>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="31">
-      <c r="A5" s="6">
+      <c r="N4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="31">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
+        <v>3267</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" ref="D5:D8" si="0">C5-E5</f>
+        <v>-4</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3271</v>
+      </c>
+      <c r="F5" s="4">
+        <f>E5-G5</f>
+        <v>-1</v>
+      </c>
+      <c r="G5" s="4">
         <v>3272</v>
       </c>
-      <c r="D5" s="6">
-        <f t="shared" ref="D5:D8" si="0">C5-E5</f>
+      <c r="H5" s="4">
+        <f t="shared" ref="H5:H8" si="1">G5-I5</f>
         <v>-10</v>
       </c>
-      <c r="E5" s="6">
+      <c r="I5" s="4">
         <v>3282</v>
       </c>
-      <c r="F5" s="6">
-        <f>E5-G5</f>
+      <c r="J5" s="4">
+        <f>I5-K5</f>
         <v>-5</v>
       </c>
-      <c r="G5" s="6">
+      <c r="K5" s="4">
         <v>3287</v>
       </c>
-      <c r="H5" s="6">
-        <f>G5-I5</f>
+      <c r="L5" s="4">
+        <f>K5-M5</f>
         <v>154</v>
       </c>
-      <c r="I5" s="6">
+      <c r="M5" s="4">
         <v>3133</v>
       </c>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="31">
-      <c r="A6" s="6">
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" ht="31">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
+        <v>41313</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>-300</v>
+      </c>
+      <c r="E6" s="4">
+        <v>41613</v>
+      </c>
+      <c r="F6" s="4">
+        <f t="shared" ref="F6:F7" si="2">E6-G6</f>
+        <v>-1491</v>
+      </c>
+      <c r="G6" s="4">
         <v>43104</v>
       </c>
-      <c r="D6" s="6">
+      <c r="H6" s="4">
+        <f t="shared" si="1"/>
+        <v>-459</v>
+      </c>
+      <c r="I6" s="4">
+        <v>43563</v>
+      </c>
+      <c r="J6" s="4">
+        <f t="shared" ref="J6:J8" si="3">I6-K6</f>
+        <v>40</v>
+      </c>
+      <c r="K6" s="4">
+        <v>43523</v>
+      </c>
+      <c r="L6" s="4">
+        <f t="shared" ref="L6:L8" si="4">K6-M6</f>
+        <v>655</v>
+      </c>
+      <c r="M6" s="4">
+        <v>42868</v>
+      </c>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" ht="31">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>609996</v>
+      </c>
+      <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>-459</v>
-      </c>
-      <c r="E6" s="6">
-        <v>43563</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" ref="F6:F8" si="1">E6-G6</f>
-        <v>40</v>
-      </c>
-      <c r="G6" s="6">
-        <v>43523</v>
-      </c>
-      <c r="H6" s="6">
-        <f t="shared" ref="H6:H8" si="2">G6-I6</f>
-        <v>655</v>
-      </c>
-      <c r="I6" s="6">
-        <v>42868</v>
-      </c>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="31">
-      <c r="A7" s="6">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6">
+        <v>-23984</v>
+      </c>
+      <c r="E7" s="4">
+        <v>633980</v>
+      </c>
+      <c r="F7" s="4">
+        <f t="shared" si="2"/>
+        <v>-24021</v>
+      </c>
+      <c r="G7" s="4">
         <v>658001</v>
       </c>
-      <c r="D7" s="6">
-        <f t="shared" si="0"/>
+      <c r="H7" s="4">
+        <f t="shared" si="1"/>
         <v>-8259</v>
       </c>
-      <c r="E7" s="6">
+      <c r="I7" s="4">
         <v>666260</v>
       </c>
-      <c r="F7" s="6">
-        <f t="shared" si="1"/>
+      <c r="J7" s="4">
+        <f t="shared" si="3"/>
         <v>-7478</v>
       </c>
-      <c r="G7" s="6">
+      <c r="K7" s="4">
         <v>673738</v>
       </c>
-      <c r="H7" s="6">
-        <f t="shared" si="2"/>
+      <c r="L7" s="4">
+        <f t="shared" si="4"/>
         <v>7083</v>
       </c>
-      <c r="I7" s="6">
+      <c r="M7" s="4">
         <v>666655</v>
       </c>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="31">
-      <c r="A8" s="5" t="s">
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="31">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="8">
+      <c r="B8" s="3"/>
+      <c r="C8" s="9">
         <f>SUM(C3:C7)</f>
-        <v>704750</v>
+        <v>654923</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
+        <v>-24314</v>
+      </c>
+      <c r="E8" s="9">
+        <f>SUM(E3:E7)</f>
+        <v>679237</v>
+      </c>
+      <c r="F8" s="9">
+        <f>SUM(F3:F7)</f>
+        <v>-25513</v>
+      </c>
+      <c r="G8" s="6">
+        <f>SUM(G3:G7)</f>
+        <v>704750</v>
+      </c>
+      <c r="H8" s="7">
+        <f t="shared" si="1"/>
         <v>-8729</v>
       </c>
-      <c r="E8" s="7">
-        <f>SUM(E3:E7)</f>
+      <c r="I8" s="5">
+        <f>SUM(I3:I7)</f>
         <v>713479</v>
       </c>
-      <c r="F8" s="7">
-        <f t="shared" si="1"/>
+      <c r="J8" s="5">
+        <f t="shared" si="3"/>
         <v>-7443</v>
       </c>
-      <c r="G8" s="7">
-        <f>SUM(G3:G7)</f>
+      <c r="K8" s="5">
+        <f>SUM(K3:K7)</f>
         <v>720922</v>
       </c>
-      <c r="H8" s="7">
-        <f t="shared" si="2"/>
+      <c r="L8" s="5">
+        <f t="shared" si="4"/>
         <v>7891</v>
       </c>
-      <c r="I8" s="7">
-        <f>SUM(I3:I7)</f>
+      <c r="M8" s="5">
+        <f>SUM(M3:M7)</f>
         <v>713031</v>
       </c>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="31">
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="31">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -782,8 +930,12 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="31">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" ht="31">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -794,8 +946,12 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="31">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" ht="31">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -806,8 +962,12 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="31">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" ht="31">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -818,14 +978,20 @@
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed some city data
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adyliu/codes/github/china_area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5C801B-7FBF-E641-95B8-469A0F8CD731}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D1D82B-D9BB-EE40-BF40-2855C4117764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15940" xr2:uid="{5888D5A7-D7A2-FC4B-8093-B0573B8EE50E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="总统计" sheetId="1" r:id="rId1"/>
+    <sheet name="分省统计" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="78">
   <si>
     <t>级别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,6 +72,210 @@
   <si>
     <t>数量</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>省</t>
+  </si>
+  <si>
+    <t>市</t>
+  </si>
+  <si>
+    <t>区/县</t>
+  </si>
+  <si>
+    <t>街道/镇</t>
+  </si>
+  <si>
+    <t>社区/村</t>
+  </si>
+  <si>
+    <t>北京市</t>
+  </si>
+  <si>
+    <t>天津市</t>
+  </si>
+  <si>
+    <t>河北省</t>
+  </si>
+  <si>
+    <t>山西省</t>
+  </si>
+  <si>
+    <t>内蒙古自治区</t>
+  </si>
+  <si>
+    <t>辽宁省</t>
+  </si>
+  <si>
+    <t>吉林省</t>
+  </si>
+  <si>
+    <t>黑龙江省</t>
+  </si>
+  <si>
+    <t>上海市</t>
+  </si>
+  <si>
+    <t>江苏省</t>
+  </si>
+  <si>
+    <t>浙江省</t>
+  </si>
+  <si>
+    <t>安徽省</t>
+  </si>
+  <si>
+    <t>福建省</t>
+  </si>
+  <si>
+    <t>江西省</t>
+  </si>
+  <si>
+    <t>山东省</t>
+  </si>
+  <si>
+    <t>河南省</t>
+  </si>
+  <si>
+    <t>湖北省</t>
+  </si>
+  <si>
+    <t>湖南省</t>
+  </si>
+  <si>
+    <t>广东省</t>
+  </si>
+  <si>
+    <t>广西壮族自治区</t>
+  </si>
+  <si>
+    <t>海南省</t>
+  </si>
+  <si>
+    <t>重庆市</t>
+  </si>
+  <si>
+    <t>四川省</t>
+  </si>
+  <si>
+    <t>贵州省</t>
+  </si>
+  <si>
+    <t>云南省</t>
+  </si>
+  <si>
+    <t>西藏自治区</t>
+  </si>
+  <si>
+    <t>陕西省</t>
+  </si>
+  <si>
+    <t>甘肃省</t>
+  </si>
+  <si>
+    <t>青海省</t>
+  </si>
+  <si>
+    <t>宁夏回族自治区</t>
+  </si>
+  <si>
+    <t>新疆维吾尔自治区</t>
+  </si>
+  <si>
+    <t>120000000000</t>
+  </si>
+  <si>
+    <t>130000000000</t>
+  </si>
+  <si>
+    <t>140000000000</t>
+  </si>
+  <si>
+    <t>150000000000</t>
+  </si>
+  <si>
+    <t>210000000000</t>
+  </si>
+  <si>
+    <t>220000000000</t>
+  </si>
+  <si>
+    <t>230000000000</t>
+  </si>
+  <si>
+    <t>310000000000</t>
+  </si>
+  <si>
+    <t>320000000000</t>
+  </si>
+  <si>
+    <t>330000000000</t>
+  </si>
+  <si>
+    <t>340000000000</t>
+  </si>
+  <si>
+    <t>350000000000</t>
+  </si>
+  <si>
+    <t>360000000000</t>
+  </si>
+  <si>
+    <t>370000000000</t>
+  </si>
+  <si>
+    <t>410000000000</t>
+  </si>
+  <si>
+    <t>420000000000</t>
+  </si>
+  <si>
+    <t>430000000000</t>
+  </si>
+  <si>
+    <t>440000000000</t>
+  </si>
+  <si>
+    <t>450000000000</t>
+  </si>
+  <si>
+    <t>460000000000</t>
+  </si>
+  <si>
+    <t>500000000000</t>
+  </si>
+  <si>
+    <t>510000000000</t>
+  </si>
+  <si>
+    <t>520000000000</t>
+  </si>
+  <si>
+    <t>530000000000</t>
+  </si>
+  <si>
+    <t>540000000000</t>
+  </si>
+  <si>
+    <t>610000000000</t>
+  </si>
+  <si>
+    <t>620000000000</t>
+  </si>
+  <si>
+    <t>630000000000</t>
+  </si>
+  <si>
+    <t>640000000000</t>
+  </si>
+  <si>
+    <t>650000000000</t>
+  </si>
+  <si>
+    <t>110000000000</t>
   </si>
 </sst>
 </file>
@@ -209,7 +414,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -250,6 +455,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -569,7 +780,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -697,11 +908,11 @@
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <v>316</v>
+        <v>342</v>
       </c>
       <c r="D4" s="4">
         <f>C4-E4</f>
-        <v>-26</v>
+        <v>0</v>
       </c>
       <c r="E4" s="4">
         <v>342</v>
@@ -875,11 +1086,11 @@
       <c r="B8" s="3"/>
       <c r="C8" s="9">
         <f>SUM(C3:C7)</f>
-        <v>654923</v>
+        <v>654949</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>-24314</v>
+        <v>-24288</v>
       </c>
       <c r="E8" s="9">
         <f>SUM(E3:E7)</f>
@@ -996,4 +1207,2954 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C34F99D-D4B0-3D47-9557-3DB9ECC9679D}">
+  <dimension ref="A1:AG34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33">
+      <c r="A1" s="15">
+        <v>2022</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15">
+        <v>2021</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15">
+        <v>2020</v>
+      </c>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15">
+        <v>2019</v>
+      </c>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="15">
+        <v>2018</v>
+      </c>
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
+    </row>
+    <row r="2" spans="1:33">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>349</v>
+      </c>
+      <c r="I3">
+        <v>168</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>339</v>
+      </c>
+      <c r="O3">
+        <v>7270</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>16</v>
+      </c>
+      <c r="T3">
+        <v>339</v>
+      </c>
+      <c r="U3">
+        <v>7169</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>16</v>
+      </c>
+      <c r="Z3">
+        <v>336</v>
+      </c>
+      <c r="AA3">
+        <v>7154</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD3">
+        <v>1</v>
+      </c>
+      <c r="AE3">
+        <v>16</v>
+      </c>
+      <c r="AF3">
+        <v>336</v>
+      </c>
+      <c r="AG3">
+        <v>7093</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33">
+      <c r="A4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>297</v>
+      </c>
+      <c r="I4">
+        <v>5573</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>16</v>
+      </c>
+      <c r="N4">
+        <v>300</v>
+      </c>
+      <c r="O4">
+        <v>5521</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>16</v>
+      </c>
+      <c r="T4">
+        <v>301</v>
+      </c>
+      <c r="U4">
+        <v>5490</v>
+      </c>
+      <c r="V4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="W4" t="s">
+        <v>17</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>16</v>
+      </c>
+      <c r="Z4">
+        <v>306</v>
+      </c>
+      <c r="AA4">
+        <v>5579</v>
+      </c>
+      <c r="AB4" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <v>16</v>
+      </c>
+      <c r="AF4">
+        <v>305</v>
+      </c>
+      <c r="AG4">
+        <v>5629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
+      <c r="A5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>201</v>
+      </c>
+      <c r="G5">
+        <v>2361</v>
+      </c>
+      <c r="I5">
+        <v>53817</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>201</v>
+      </c>
+      <c r="N5">
+        <v>2363</v>
+      </c>
+      <c r="O5">
+        <v>53850</v>
+      </c>
+      <c r="P5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5">
+        <v>11</v>
+      </c>
+      <c r="S5">
+        <v>202</v>
+      </c>
+      <c r="T5">
+        <v>2357</v>
+      </c>
+      <c r="U5">
+        <v>53609</v>
+      </c>
+      <c r="V5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="W5" t="s">
+        <v>18</v>
+      </c>
+      <c r="X5">
+        <v>11</v>
+      </c>
+      <c r="Y5">
+        <v>202</v>
+      </c>
+      <c r="Z5">
+        <v>2355</v>
+      </c>
+      <c r="AA5">
+        <v>53463</v>
+      </c>
+      <c r="AB5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD5">
+        <v>11</v>
+      </c>
+      <c r="AE5">
+        <v>202</v>
+      </c>
+      <c r="AF5">
+        <v>2348</v>
+      </c>
+      <c r="AG5">
+        <v>53247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33">
+      <c r="A6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>133</v>
+      </c>
+      <c r="G6">
+        <v>1358</v>
+      </c>
+      <c r="I6">
+        <v>21865</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6">
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <v>133</v>
+      </c>
+      <c r="N6">
+        <v>1491</v>
+      </c>
+      <c r="O6">
+        <v>23465</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6">
+        <v>11</v>
+      </c>
+      <c r="S6">
+        <v>133</v>
+      </c>
+      <c r="T6">
+        <v>1488</v>
+      </c>
+      <c r="U6">
+        <v>27966</v>
+      </c>
+      <c r="V6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="W6" t="s">
+        <v>19</v>
+      </c>
+      <c r="X6">
+        <v>11</v>
+      </c>
+      <c r="Y6">
+        <v>133</v>
+      </c>
+      <c r="Z6">
+        <v>1485</v>
+      </c>
+      <c r="AA6">
+        <v>29683</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD6">
+        <v>11</v>
+      </c>
+      <c r="AE6">
+        <v>136</v>
+      </c>
+      <c r="AF6">
+        <v>1482</v>
+      </c>
+      <c r="AG6">
+        <v>30328</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33">
+      <c r="A7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>117</v>
+      </c>
+      <c r="G7">
+        <v>1228</v>
+      </c>
+      <c r="I7">
+        <v>14467</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>117</v>
+      </c>
+      <c r="N7">
+        <v>1232</v>
+      </c>
+      <c r="O7">
+        <v>14426</v>
+      </c>
+      <c r="P7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R7">
+        <v>12</v>
+      </c>
+      <c r="S7">
+        <v>118</v>
+      </c>
+      <c r="T7">
+        <v>1248</v>
+      </c>
+      <c r="U7">
+        <v>14489</v>
+      </c>
+      <c r="V7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="W7" t="s">
+        <v>20</v>
+      </c>
+      <c r="X7">
+        <v>12</v>
+      </c>
+      <c r="Y7">
+        <v>118</v>
+      </c>
+      <c r="Z7">
+        <v>1272</v>
+      </c>
+      <c r="AA7">
+        <v>14592</v>
+      </c>
+      <c r="AB7" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD7">
+        <v>12</v>
+      </c>
+      <c r="AE7">
+        <v>118</v>
+      </c>
+      <c r="AF7">
+        <v>1268</v>
+      </c>
+      <c r="AG7">
+        <v>14543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33">
+      <c r="A8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>114</v>
+      </c>
+      <c r="G8">
+        <v>1404</v>
+      </c>
+      <c r="I8">
+        <v>16399</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8">
+        <v>14</v>
+      </c>
+      <c r="M8">
+        <v>114</v>
+      </c>
+      <c r="N8">
+        <v>1406</v>
+      </c>
+      <c r="O8">
+        <v>16376</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>21</v>
+      </c>
+      <c r="R8">
+        <v>14</v>
+      </c>
+      <c r="S8">
+        <v>114</v>
+      </c>
+      <c r="T8">
+        <v>1581</v>
+      </c>
+      <c r="U8">
+        <v>16418</v>
+      </c>
+      <c r="V8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="W8" t="s">
+        <v>21</v>
+      </c>
+      <c r="X8">
+        <v>14</v>
+      </c>
+      <c r="Y8">
+        <v>114</v>
+      </c>
+      <c r="Z8">
+        <v>1586</v>
+      </c>
+      <c r="AA8">
+        <v>16351</v>
+      </c>
+      <c r="AB8" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD8">
+        <v>14</v>
+      </c>
+      <c r="AE8">
+        <v>114</v>
+      </c>
+      <c r="AF8">
+        <v>1590</v>
+      </c>
+      <c r="AG8">
+        <v>16275</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33">
+      <c r="A9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>77</v>
+      </c>
+      <c r="G9">
+        <v>1059</v>
+      </c>
+      <c r="I9">
+        <v>11755</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9">
+        <v>9</v>
+      </c>
+      <c r="M9">
+        <v>77</v>
+      </c>
+      <c r="N9">
+        <v>1048</v>
+      </c>
+      <c r="O9">
+        <v>11727</v>
+      </c>
+      <c r="P9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9">
+        <v>9</v>
+      </c>
+      <c r="S9">
+        <v>77</v>
+      </c>
+      <c r="T9">
+        <v>1044</v>
+      </c>
+      <c r="U9">
+        <v>11683</v>
+      </c>
+      <c r="V9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="W9" t="s">
+        <v>22</v>
+      </c>
+      <c r="X9">
+        <v>9</v>
+      </c>
+      <c r="Y9">
+        <v>77</v>
+      </c>
+      <c r="Z9">
+        <v>1045</v>
+      </c>
+      <c r="AA9">
+        <v>11647</v>
+      </c>
+      <c r="AB9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD9">
+        <v>9</v>
+      </c>
+      <c r="AE9">
+        <v>77</v>
+      </c>
+      <c r="AF9">
+        <v>1038</v>
+      </c>
+      <c r="AG9">
+        <v>11618</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33">
+      <c r="A10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>139</v>
+      </c>
+      <c r="G10">
+        <v>1728</v>
+      </c>
+      <c r="I10">
+        <v>13919</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10">
+        <v>13</v>
+      </c>
+      <c r="M10">
+        <v>139</v>
+      </c>
+      <c r="N10">
+        <v>1727</v>
+      </c>
+      <c r="O10">
+        <v>13879</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10">
+        <v>13</v>
+      </c>
+      <c r="S10">
+        <v>139</v>
+      </c>
+      <c r="T10">
+        <v>1919</v>
+      </c>
+      <c r="U10">
+        <v>14049</v>
+      </c>
+      <c r="V10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="W10" t="s">
+        <v>23</v>
+      </c>
+      <c r="X10">
+        <v>13</v>
+      </c>
+      <c r="Y10">
+        <v>146</v>
+      </c>
+      <c r="Z10">
+        <v>1990</v>
+      </c>
+      <c r="AA10">
+        <v>14115</v>
+      </c>
+      <c r="AB10" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD10">
+        <v>13</v>
+      </c>
+      <c r="AE10">
+        <v>146</v>
+      </c>
+      <c r="AF10">
+        <v>1971</v>
+      </c>
+      <c r="AG10">
+        <v>14093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33">
+      <c r="A11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>234</v>
+      </c>
+      <c r="I11">
+        <v>6234</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>16</v>
+      </c>
+      <c r="N11">
+        <v>234</v>
+      </c>
+      <c r="O11">
+        <v>6188</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>24</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11">
+        <v>16</v>
+      </c>
+      <c r="T11">
+        <v>234</v>
+      </c>
+      <c r="U11">
+        <v>6089</v>
+      </c>
+      <c r="V11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="W11" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>16</v>
+      </c>
+      <c r="Z11">
+        <v>234</v>
+      </c>
+      <c r="AA11">
+        <v>6013</v>
+      </c>
+      <c r="AB11" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD11">
+        <v>1</v>
+      </c>
+      <c r="AE11">
+        <v>16</v>
+      </c>
+      <c r="AF11">
+        <v>234</v>
+      </c>
+      <c r="AG11">
+        <v>5925</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33">
+      <c r="A12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>119</v>
+      </c>
+      <c r="G12">
+        <v>1497</v>
+      </c>
+      <c r="I12">
+        <v>21946</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <v>13</v>
+      </c>
+      <c r="M12">
+        <v>120</v>
+      </c>
+      <c r="N12">
+        <v>1520</v>
+      </c>
+      <c r="O12">
+        <v>22180</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>25</v>
+      </c>
+      <c r="R12">
+        <v>13</v>
+      </c>
+      <c r="S12">
+        <v>120</v>
+      </c>
+      <c r="T12">
+        <v>1533</v>
+      </c>
+      <c r="U12">
+        <v>22176</v>
+      </c>
+      <c r="V12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="W12" t="s">
+        <v>25</v>
+      </c>
+      <c r="X12">
+        <v>13</v>
+      </c>
+      <c r="Y12">
+        <v>120</v>
+      </c>
+      <c r="Z12">
+        <v>1549</v>
+      </c>
+      <c r="AA12">
+        <v>22312</v>
+      </c>
+      <c r="AB12" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD12">
+        <v>13</v>
+      </c>
+      <c r="AE12">
+        <v>120</v>
+      </c>
+      <c r="AF12">
+        <v>1568</v>
+      </c>
+      <c r="AG12">
+        <v>22226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33">
+      <c r="A13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>102</v>
+      </c>
+      <c r="G13">
+        <v>1384</v>
+      </c>
+      <c r="I13">
+        <v>25306</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13">
+        <v>11</v>
+      </c>
+      <c r="M13">
+        <v>102</v>
+      </c>
+      <c r="N13">
+        <v>1384</v>
+      </c>
+      <c r="O13">
+        <v>25527</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>26</v>
+      </c>
+      <c r="R13">
+        <v>11</v>
+      </c>
+      <c r="S13">
+        <v>102</v>
+      </c>
+      <c r="T13">
+        <v>1386</v>
+      </c>
+      <c r="U13">
+        <v>25619</v>
+      </c>
+      <c r="V13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="W13" t="s">
+        <v>26</v>
+      </c>
+      <c r="X13">
+        <v>11</v>
+      </c>
+      <c r="Y13">
+        <v>101</v>
+      </c>
+      <c r="Z13">
+        <v>1396</v>
+      </c>
+      <c r="AA13">
+        <v>30626</v>
+      </c>
+      <c r="AB13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD13">
+        <v>11</v>
+      </c>
+      <c r="AE13">
+        <v>101</v>
+      </c>
+      <c r="AF13">
+        <v>1400</v>
+      </c>
+      <c r="AG13">
+        <v>32121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33">
+      <c r="A14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>135</v>
+      </c>
+      <c r="G14">
+        <v>1661</v>
+      </c>
+      <c r="I14">
+        <v>18236</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14">
+        <v>16</v>
+      </c>
+      <c r="M14">
+        <v>136</v>
+      </c>
+      <c r="N14">
+        <v>1661</v>
+      </c>
+      <c r="O14">
+        <v>18306</v>
+      </c>
+      <c r="P14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14">
+        <v>16</v>
+      </c>
+      <c r="S14">
+        <v>136</v>
+      </c>
+      <c r="T14">
+        <v>1636</v>
+      </c>
+      <c r="U14">
+        <v>18246</v>
+      </c>
+      <c r="V14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="W14" t="s">
+        <v>27</v>
+      </c>
+      <c r="X14">
+        <v>16</v>
+      </c>
+      <c r="Y14">
+        <v>136</v>
+      </c>
+      <c r="Z14">
+        <v>1645</v>
+      </c>
+      <c r="AA14">
+        <v>18265</v>
+      </c>
+      <c r="AB14" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD14">
+        <v>16</v>
+      </c>
+      <c r="AE14">
+        <v>136</v>
+      </c>
+      <c r="AF14">
+        <v>1645</v>
+      </c>
+      <c r="AG14">
+        <v>18300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="A15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>93</v>
+      </c>
+      <c r="G15">
+        <v>1165</v>
+      </c>
+      <c r="I15">
+        <v>17375</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15">
+        <v>9</v>
+      </c>
+      <c r="M15">
+        <v>94</v>
+      </c>
+      <c r="N15">
+        <v>1166</v>
+      </c>
+      <c r="O15">
+        <v>17288</v>
+      </c>
+      <c r="P15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>28</v>
+      </c>
+      <c r="R15">
+        <v>9</v>
+      </c>
+      <c r="S15">
+        <v>94</v>
+      </c>
+      <c r="T15">
+        <v>1166</v>
+      </c>
+      <c r="U15">
+        <v>17252</v>
+      </c>
+      <c r="V15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="W15" t="s">
+        <v>28</v>
+      </c>
+      <c r="X15">
+        <v>9</v>
+      </c>
+      <c r="Y15">
+        <v>94</v>
+      </c>
+      <c r="Z15">
+        <v>1175</v>
+      </c>
+      <c r="AA15">
+        <v>17172</v>
+      </c>
+      <c r="AB15" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD15">
+        <v>9</v>
+      </c>
+      <c r="AE15">
+        <v>94</v>
+      </c>
+      <c r="AF15">
+        <v>1185</v>
+      </c>
+      <c r="AG15">
+        <v>17080</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33">
+      <c r="A16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>111</v>
+      </c>
+      <c r="G16">
+        <v>1771</v>
+      </c>
+      <c r="I16">
+        <v>21778</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="K16" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16">
+        <v>11</v>
+      </c>
+      <c r="M16">
+        <v>111</v>
+      </c>
+      <c r="N16">
+        <v>1771</v>
+      </c>
+      <c r="O16">
+        <v>21616</v>
+      </c>
+      <c r="P16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16">
+        <v>11</v>
+      </c>
+      <c r="S16">
+        <v>111</v>
+      </c>
+      <c r="T16">
+        <v>1783</v>
+      </c>
+      <c r="U16">
+        <v>21598</v>
+      </c>
+      <c r="V16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="W16" t="s">
+        <v>29</v>
+      </c>
+      <c r="X16">
+        <v>11</v>
+      </c>
+      <c r="Y16">
+        <v>111</v>
+      </c>
+      <c r="Z16">
+        <v>1783</v>
+      </c>
+      <c r="AA16">
+        <v>21451</v>
+      </c>
+      <c r="AB16" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD16">
+        <v>11</v>
+      </c>
+      <c r="AE16">
+        <v>111</v>
+      </c>
+      <c r="AF16">
+        <v>1783</v>
+      </c>
+      <c r="AG16">
+        <v>21367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="A17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>169</v>
+      </c>
+      <c r="G17">
+        <v>1853</v>
+      </c>
+      <c r="I17">
+        <v>62081</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17">
+        <v>16</v>
+      </c>
+      <c r="M17">
+        <v>169</v>
+      </c>
+      <c r="N17">
+        <v>1860</v>
+      </c>
+      <c r="O17">
+        <v>75093</v>
+      </c>
+      <c r="P17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>30</v>
+      </c>
+      <c r="R17">
+        <v>16</v>
+      </c>
+      <c r="S17">
+        <v>172</v>
+      </c>
+      <c r="T17">
+        <v>1862</v>
+      </c>
+      <c r="U17">
+        <v>77299</v>
+      </c>
+      <c r="V17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="W17" t="s">
+        <v>30</v>
+      </c>
+      <c r="X17">
+        <v>17</v>
+      </c>
+      <c r="Y17">
+        <v>173</v>
+      </c>
+      <c r="Z17">
+        <v>1859</v>
+      </c>
+      <c r="AA17">
+        <v>77976</v>
+      </c>
+      <c r="AB17" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD17">
+        <v>17</v>
+      </c>
+      <c r="AE17">
+        <v>174</v>
+      </c>
+      <c r="AF17">
+        <v>1851</v>
+      </c>
+      <c r="AG17">
+        <v>81230</v>
+      </c>
+    </row>
+    <row r="18" spans="1:33">
+      <c r="A18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <v>18</v>
+      </c>
+      <c r="E18">
+        <v>198</v>
+      </c>
+      <c r="G18">
+        <v>2542</v>
+      </c>
+      <c r="I18">
+        <v>51218</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18">
+        <v>18</v>
+      </c>
+      <c r="M18">
+        <v>199</v>
+      </c>
+      <c r="N18">
+        <v>2581</v>
+      </c>
+      <c r="O18">
+        <v>52331</v>
+      </c>
+      <c r="P18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>31</v>
+      </c>
+      <c r="R18">
+        <v>18</v>
+      </c>
+      <c r="S18">
+        <v>199</v>
+      </c>
+      <c r="T18">
+        <v>2577</v>
+      </c>
+      <c r="U18">
+        <v>52123</v>
+      </c>
+      <c r="V18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="W18" t="s">
+        <v>31</v>
+      </c>
+      <c r="X18">
+        <v>18</v>
+      </c>
+      <c r="Y18">
+        <v>199</v>
+      </c>
+      <c r="Z18">
+        <v>2567</v>
+      </c>
+      <c r="AA18">
+        <v>52054</v>
+      </c>
+      <c r="AB18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD18">
+        <v>18</v>
+      </c>
+      <c r="AE18">
+        <v>199</v>
+      </c>
+      <c r="AF18">
+        <v>2566</v>
+      </c>
+      <c r="AG18">
+        <v>52047</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33">
+      <c r="A19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>117</v>
+      </c>
+      <c r="G19">
+        <v>1487</v>
+      </c>
+      <c r="I19">
+        <v>27713</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19">
+        <v>14</v>
+      </c>
+      <c r="M19">
+        <v>117</v>
+      </c>
+      <c r="N19">
+        <v>1483</v>
+      </c>
+      <c r="O19">
+        <v>28380</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19">
+        <v>14</v>
+      </c>
+      <c r="S19">
+        <v>117</v>
+      </c>
+      <c r="T19">
+        <v>1478</v>
+      </c>
+      <c r="U19">
+        <v>28547</v>
+      </c>
+      <c r="V19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="W19" t="s">
+        <v>32</v>
+      </c>
+      <c r="X19">
+        <v>14</v>
+      </c>
+      <c r="Y19">
+        <v>117</v>
+      </c>
+      <c r="Z19">
+        <v>1488</v>
+      </c>
+      <c r="AA19">
+        <v>28867</v>
+      </c>
+      <c r="AB19" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD19">
+        <v>14</v>
+      </c>
+      <c r="AE19">
+        <v>117</v>
+      </c>
+      <c r="AF19">
+        <v>1484</v>
+      </c>
+      <c r="AG19">
+        <v>29718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33">
+      <c r="A20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+      <c r="E20">
+        <v>149</v>
+      </c>
+      <c r="G20">
+        <v>2008</v>
+      </c>
+      <c r="I20">
+        <v>29499</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20">
+        <v>14</v>
+      </c>
+      <c r="M20">
+        <v>150</v>
+      </c>
+      <c r="N20">
+        <v>2006</v>
+      </c>
+      <c r="O20">
+        <v>29479</v>
+      </c>
+      <c r="P20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>33</v>
+      </c>
+      <c r="R20">
+        <v>14</v>
+      </c>
+      <c r="S20">
+        <v>151</v>
+      </c>
+      <c r="T20">
+        <v>2008</v>
+      </c>
+      <c r="U20">
+        <v>29454</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="W20" t="s">
+        <v>33</v>
+      </c>
+      <c r="X20">
+        <v>14</v>
+      </c>
+      <c r="Y20">
+        <v>152</v>
+      </c>
+      <c r="Z20">
+        <v>2006</v>
+      </c>
+      <c r="AA20">
+        <v>29391</v>
+      </c>
+      <c r="AB20" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD20">
+        <v>14</v>
+      </c>
+      <c r="AE20">
+        <v>152</v>
+      </c>
+      <c r="AF20">
+        <v>2002</v>
+      </c>
+      <c r="AG20">
+        <v>29365</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="A21" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>141</v>
+      </c>
+      <c r="G21">
+        <v>1760</v>
+      </c>
+      <c r="I21">
+        <v>26735</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21">
+        <v>21</v>
+      </c>
+      <c r="M21">
+        <v>141</v>
+      </c>
+      <c r="N21">
+        <v>1765</v>
+      </c>
+      <c r="O21">
+        <v>26631</v>
+      </c>
+      <c r="P21" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21">
+        <v>21</v>
+      </c>
+      <c r="S21">
+        <v>141</v>
+      </c>
+      <c r="T21">
+        <v>1759</v>
+      </c>
+      <c r="U21">
+        <v>26593</v>
+      </c>
+      <c r="V21" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="W21" t="s">
+        <v>34</v>
+      </c>
+      <c r="X21">
+        <v>21</v>
+      </c>
+      <c r="Y21">
+        <v>141</v>
+      </c>
+      <c r="Z21">
+        <v>1776</v>
+      </c>
+      <c r="AA21">
+        <v>26513</v>
+      </c>
+      <c r="AB21" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD21">
+        <v>21</v>
+      </c>
+      <c r="AE21">
+        <v>140</v>
+      </c>
+      <c r="AF21">
+        <v>1778</v>
+      </c>
+      <c r="AG21">
+        <v>26467</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="A22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>125</v>
+      </c>
+      <c r="G22">
+        <v>1282</v>
+      </c>
+      <c r="I22">
+        <v>16610</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22">
+        <v>14</v>
+      </c>
+      <c r="M22">
+        <v>125</v>
+      </c>
+      <c r="N22">
+        <v>1279</v>
+      </c>
+      <c r="O22">
+        <v>16550</v>
+      </c>
+      <c r="P22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>35</v>
+      </c>
+      <c r="R22">
+        <v>14</v>
+      </c>
+      <c r="S22">
+        <v>125</v>
+      </c>
+      <c r="T22">
+        <v>1279</v>
+      </c>
+      <c r="U22">
+        <v>16496</v>
+      </c>
+      <c r="V22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="W22" t="s">
+        <v>35</v>
+      </c>
+      <c r="X22">
+        <v>14</v>
+      </c>
+      <c r="Y22">
+        <v>125</v>
+      </c>
+      <c r="Z22">
+        <v>1291</v>
+      </c>
+      <c r="AA22">
+        <v>16457</v>
+      </c>
+      <c r="AB22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD22">
+        <v>14</v>
+      </c>
+      <c r="AE22">
+        <v>125</v>
+      </c>
+      <c r="AF22">
+        <v>1291</v>
+      </c>
+      <c r="AG22">
+        <v>16462</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="A23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>28</v>
+      </c>
+      <c r="G23">
+        <v>244</v>
+      </c>
+      <c r="I23">
+        <v>3294</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="K23" t="s">
+        <v>36</v>
+      </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
+      <c r="M23">
+        <v>28</v>
+      </c>
+      <c r="N23">
+        <v>244</v>
+      </c>
+      <c r="O23">
+        <v>3315</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>36</v>
+      </c>
+      <c r="R23">
+        <v>5</v>
+      </c>
+      <c r="S23">
+        <v>28</v>
+      </c>
+      <c r="T23">
+        <v>244</v>
+      </c>
+      <c r="U23">
+        <v>3332</v>
+      </c>
+      <c r="V23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="W23" t="s">
+        <v>36</v>
+      </c>
+      <c r="X23">
+        <v>5</v>
+      </c>
+      <c r="Y23">
+        <v>28</v>
+      </c>
+      <c r="Z23">
+        <v>244</v>
+      </c>
+      <c r="AA23">
+        <v>3333</v>
+      </c>
+      <c r="AB23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD23">
+        <v>5</v>
+      </c>
+      <c r="AE23">
+        <v>28</v>
+      </c>
+      <c r="AF23">
+        <v>244</v>
+      </c>
+      <c r="AG23">
+        <v>3343</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33">
+      <c r="A24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>38</v>
+      </c>
+      <c r="G24">
+        <v>1031</v>
+      </c>
+      <c r="I24">
+        <v>11234</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="K24" t="s">
+        <v>37</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>38</v>
+      </c>
+      <c r="N24">
+        <v>1029</v>
+      </c>
+      <c r="O24">
+        <v>11224</v>
+      </c>
+      <c r="P24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>37</v>
+      </c>
+      <c r="R24">
+        <v>2</v>
+      </c>
+      <c r="S24">
+        <v>38</v>
+      </c>
+      <c r="T24">
+        <v>1028</v>
+      </c>
+      <c r="U24">
+        <v>11206</v>
+      </c>
+      <c r="V24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="W24" t="s">
+        <v>37</v>
+      </c>
+      <c r="X24">
+        <v>2</v>
+      </c>
+      <c r="Y24">
+        <v>38</v>
+      </c>
+      <c r="Z24">
+        <v>1033</v>
+      </c>
+      <c r="AA24">
+        <v>11204</v>
+      </c>
+      <c r="AB24" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD24">
+        <v>2</v>
+      </c>
+      <c r="AE24">
+        <v>38</v>
+      </c>
+      <c r="AF24">
+        <v>1032</v>
+      </c>
+      <c r="AG24">
+        <v>11189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33">
+      <c r="A25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25">
+        <v>21</v>
+      </c>
+      <c r="E25">
+        <v>204</v>
+      </c>
+      <c r="G25">
+        <v>3111</v>
+      </c>
+      <c r="I25">
+        <v>34403</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" t="s">
+        <v>38</v>
+      </c>
+      <c r="L25">
+        <v>21</v>
+      </c>
+      <c r="M25">
+        <v>204</v>
+      </c>
+      <c r="N25">
+        <v>3240</v>
+      </c>
+      <c r="O25">
+        <v>35425</v>
+      </c>
+      <c r="P25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>38</v>
+      </c>
+      <c r="R25">
+        <v>21</v>
+      </c>
+      <c r="S25">
+        <v>204</v>
+      </c>
+      <c r="T25">
+        <v>4346</v>
+      </c>
+      <c r="U25">
+        <v>53191</v>
+      </c>
+      <c r="V25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="W25" t="s">
+        <v>38</v>
+      </c>
+      <c r="X25">
+        <v>21</v>
+      </c>
+      <c r="Y25">
+        <v>204</v>
+      </c>
+      <c r="Z25">
+        <v>4642</v>
+      </c>
+      <c r="AA25">
+        <v>53578</v>
+      </c>
+      <c r="AB25" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD25">
+        <v>21</v>
+      </c>
+      <c r="AE25">
+        <v>204</v>
+      </c>
+      <c r="AF25">
+        <v>4647</v>
+      </c>
+      <c r="AG25">
+        <v>53828</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33">
+      <c r="A26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>93</v>
+      </c>
+      <c r="G26">
+        <v>1511</v>
+      </c>
+      <c r="I26">
+        <v>17920</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26">
+        <v>9</v>
+      </c>
+      <c r="M26">
+        <v>93</v>
+      </c>
+      <c r="N26">
+        <v>1506</v>
+      </c>
+      <c r="O26">
+        <v>17862</v>
+      </c>
+      <c r="P26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>39</v>
+      </c>
+      <c r="R26">
+        <v>9</v>
+      </c>
+      <c r="S26">
+        <v>93</v>
+      </c>
+      <c r="T26">
+        <v>1514</v>
+      </c>
+      <c r="U26">
+        <v>17696</v>
+      </c>
+      <c r="V26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="W26" t="s">
+        <v>39</v>
+      </c>
+      <c r="X26">
+        <v>9</v>
+      </c>
+      <c r="Y26">
+        <v>93</v>
+      </c>
+      <c r="Z26">
+        <v>1482</v>
+      </c>
+      <c r="AA26">
+        <v>17547</v>
+      </c>
+      <c r="AB26" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD26">
+        <v>9</v>
+      </c>
+      <c r="AE26">
+        <v>93</v>
+      </c>
+      <c r="AF26">
+        <v>1481</v>
+      </c>
+      <c r="AG26">
+        <v>18738</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33">
+      <c r="A27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="E27">
+        <v>137</v>
+      </c>
+      <c r="G27">
+        <v>1458</v>
+      </c>
+      <c r="I27">
+        <v>14771</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27">
+        <v>16</v>
+      </c>
+      <c r="M27">
+        <v>137</v>
+      </c>
+      <c r="N27">
+        <v>1453</v>
+      </c>
+      <c r="O27">
+        <v>14640</v>
+      </c>
+      <c r="P27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>40</v>
+      </c>
+      <c r="R27">
+        <v>16</v>
+      </c>
+      <c r="S27">
+        <v>137</v>
+      </c>
+      <c r="T27">
+        <v>1446</v>
+      </c>
+      <c r="U27">
+        <v>14575</v>
+      </c>
+      <c r="V27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="W27" t="s">
+        <v>40</v>
+      </c>
+      <c r="X27">
+        <v>16</v>
+      </c>
+      <c r="Y27">
+        <v>137</v>
+      </c>
+      <c r="Z27">
+        <v>1442</v>
+      </c>
+      <c r="AA27">
+        <v>14451</v>
+      </c>
+      <c r="AB27" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD27">
+        <v>16</v>
+      </c>
+      <c r="AE27">
+        <v>137</v>
+      </c>
+      <c r="AF27">
+        <v>1440</v>
+      </c>
+      <c r="AG27">
+        <v>14393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
+      <c r="A28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>80</v>
+      </c>
+      <c r="G28">
+        <v>701</v>
+      </c>
+      <c r="I28">
+        <v>5557</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28">
+        <v>7</v>
+      </c>
+      <c r="M28">
+        <v>80</v>
+      </c>
+      <c r="N28">
+        <v>701</v>
+      </c>
+      <c r="O28">
+        <v>5513</v>
+      </c>
+      <c r="P28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>41</v>
+      </c>
+      <c r="R28">
+        <v>7</v>
+      </c>
+      <c r="S28">
+        <v>80</v>
+      </c>
+      <c r="T28">
+        <v>701</v>
+      </c>
+      <c r="U28">
+        <v>5486</v>
+      </c>
+      <c r="V28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="W28" t="s">
+        <v>41</v>
+      </c>
+      <c r="X28">
+        <v>7</v>
+      </c>
+      <c r="Y28">
+        <v>80</v>
+      </c>
+      <c r="Z28">
+        <v>701</v>
+      </c>
+      <c r="AA28">
+        <v>5479</v>
+      </c>
+      <c r="AB28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD28">
+        <v>7</v>
+      </c>
+      <c r="AE28">
+        <v>80</v>
+      </c>
+      <c r="AF28">
+        <v>701</v>
+      </c>
+      <c r="AG28">
+        <v>5473</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
+      <c r="A29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <v>117</v>
+      </c>
+      <c r="G29">
+        <v>1336</v>
+      </c>
+      <c r="I29">
+        <v>20154</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K29" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29">
+        <v>10</v>
+      </c>
+      <c r="M29">
+        <v>117</v>
+      </c>
+      <c r="N29">
+        <v>1333</v>
+      </c>
+      <c r="O29">
+        <v>19916</v>
+      </c>
+      <c r="P29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>42</v>
+      </c>
+      <c r="R29">
+        <v>10</v>
+      </c>
+      <c r="S29">
+        <v>117</v>
+      </c>
+      <c r="T29">
+        <v>1332</v>
+      </c>
+      <c r="U29">
+        <v>19983</v>
+      </c>
+      <c r="V29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="W29" t="s">
+        <v>42</v>
+      </c>
+      <c r="X29">
+        <v>10</v>
+      </c>
+      <c r="Y29">
+        <v>117</v>
+      </c>
+      <c r="Z29">
+        <v>1334</v>
+      </c>
+      <c r="AA29">
+        <v>20515</v>
+      </c>
+      <c r="AB29" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD29">
+        <v>10</v>
+      </c>
+      <c r="AE29">
+        <v>117</v>
+      </c>
+      <c r="AF29">
+        <v>1319</v>
+      </c>
+      <c r="AG29">
+        <v>21288</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
+      <c r="A30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30">
+        <v>14</v>
+      </c>
+      <c r="E30">
+        <v>99</v>
+      </c>
+      <c r="G30">
+        <v>1405</v>
+      </c>
+      <c r="I30">
+        <v>17614</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K30" t="s">
+        <v>43</v>
+      </c>
+      <c r="L30">
+        <v>14</v>
+      </c>
+      <c r="M30">
+        <v>99</v>
+      </c>
+      <c r="N30">
+        <v>1403</v>
+      </c>
+      <c r="O30">
+        <v>17656</v>
+      </c>
+      <c r="P30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>43</v>
+      </c>
+      <c r="R30">
+        <v>14</v>
+      </c>
+      <c r="S30">
+        <v>99</v>
+      </c>
+      <c r="T30">
+        <v>1425</v>
+      </c>
+      <c r="U30">
+        <v>17633</v>
+      </c>
+      <c r="V30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="W30" t="s">
+        <v>43</v>
+      </c>
+      <c r="X30">
+        <v>14</v>
+      </c>
+      <c r="Y30">
+        <v>99</v>
+      </c>
+      <c r="Z30">
+        <v>1432</v>
+      </c>
+      <c r="AA30">
+        <v>17647</v>
+      </c>
+      <c r="AB30" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD30">
+        <v>14</v>
+      </c>
+      <c r="AE30">
+        <v>100</v>
+      </c>
+      <c r="AF30">
+        <v>1435</v>
+      </c>
+      <c r="AG30">
+        <v>17618</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33">
+      <c r="A31" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+      <c r="E31">
+        <v>46</v>
+      </c>
+      <c r="G31">
+        <v>422</v>
+      </c>
+      <c r="I31">
+        <v>4717</v>
+      </c>
+      <c r="J31" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K31" t="s">
+        <v>44</v>
+      </c>
+      <c r="L31">
+        <v>8</v>
+      </c>
+      <c r="M31">
+        <v>46</v>
+      </c>
+      <c r="N31">
+        <v>422</v>
+      </c>
+      <c r="O31">
+        <v>4706</v>
+      </c>
+      <c r="P31" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>44</v>
+      </c>
+      <c r="R31">
+        <v>8</v>
+      </c>
+      <c r="S31">
+        <v>46</v>
+      </c>
+      <c r="T31">
+        <v>422</v>
+      </c>
+      <c r="U31">
+        <v>4716</v>
+      </c>
+      <c r="V31" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="W31" t="s">
+        <v>44</v>
+      </c>
+      <c r="X31">
+        <v>8</v>
+      </c>
+      <c r="Y31">
+        <v>46</v>
+      </c>
+      <c r="Z31">
+        <v>430</v>
+      </c>
+      <c r="AA31">
+        <v>4707</v>
+      </c>
+      <c r="AB31" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD31">
+        <v>8</v>
+      </c>
+      <c r="AE31">
+        <v>47</v>
+      </c>
+      <c r="AF31">
+        <v>430</v>
+      </c>
+      <c r="AG31">
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33">
+      <c r="A32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>27</v>
+      </c>
+      <c r="G32">
+        <v>259</v>
+      </c>
+      <c r="I32">
+        <v>2900</v>
+      </c>
+      <c r="J32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K32" t="s">
+        <v>45</v>
+      </c>
+      <c r="L32">
+        <v>5</v>
+      </c>
+      <c r="M32">
+        <v>27</v>
+      </c>
+      <c r="N32">
+        <v>258</v>
+      </c>
+      <c r="O32">
+        <v>2849</v>
+      </c>
+      <c r="P32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>45</v>
+      </c>
+      <c r="R32">
+        <v>5</v>
+      </c>
+      <c r="S32">
+        <v>27</v>
+      </c>
+      <c r="T32">
+        <v>260</v>
+      </c>
+      <c r="U32">
+        <v>2841</v>
+      </c>
+      <c r="V32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="W32" t="s">
+        <v>45</v>
+      </c>
+      <c r="X32">
+        <v>5</v>
+      </c>
+      <c r="Y32">
+        <v>27</v>
+      </c>
+      <c r="Z32">
+        <v>263</v>
+      </c>
+      <c r="AA32">
+        <v>2874</v>
+      </c>
+      <c r="AB32" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD32">
+        <v>5</v>
+      </c>
+      <c r="AE32">
+        <v>27</v>
+      </c>
+      <c r="AF32">
+        <v>265</v>
+      </c>
+      <c r="AG32">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33">
+      <c r="A33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="B33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C33">
+        <v>15</v>
+      </c>
+      <c r="E33">
+        <v>110</v>
+      </c>
+      <c r="G33">
+        <v>1407</v>
+      </c>
+      <c r="I33">
+        <v>14738</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33" t="s">
+        <v>46</v>
+      </c>
+      <c r="L33">
+        <v>15</v>
+      </c>
+      <c r="M33">
+        <v>109</v>
+      </c>
+      <c r="N33">
+        <v>1408</v>
+      </c>
+      <c r="O33">
+        <v>14791</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>46</v>
+      </c>
+      <c r="R33">
+        <v>15</v>
+      </c>
+      <c r="S33">
+        <v>104</v>
+      </c>
+      <c r="T33">
+        <v>1408</v>
+      </c>
+      <c r="U33">
+        <v>14977</v>
+      </c>
+      <c r="V33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="W33" t="s">
+        <v>46</v>
+      </c>
+      <c r="X33">
+        <v>15</v>
+      </c>
+      <c r="Y33">
+        <v>106</v>
+      </c>
+      <c r="Z33">
+        <v>1416</v>
+      </c>
+      <c r="AA33">
+        <v>15244</v>
+      </c>
+      <c r="AB33" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD33">
+        <v>15</v>
+      </c>
+      <c r="AE33">
+        <v>106</v>
+      </c>
+      <c r="AF33">
+        <v>1404</v>
+      </c>
+      <c r="AG33">
+        <v>15126</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33">
+      <c r="A34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="P34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="AB34" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="V1:AA1"/>
+    <mergeCell ref="AB1:AG1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update data to 2022.10.31
</commit_message>
<xml_diff>
--- a/summary.xlsx
+++ b/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adyliu/codes/github/china_area/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adyliu/lab/china_area/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DB1A81-A960-ED46-B5A7-6B6876114C29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457EE880-D794-8241-9D5C-87C25F7B81D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="15940" activeTab="1" xr2:uid="{5888D5A7-D7A2-FC4B-8093-B0573B8EE50E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="22960" xr2:uid="{5888D5A7-D7A2-FC4B-8093-B0573B8EE50E}"/>
   </bookViews>
   <sheets>
     <sheet name="总统计" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
   <si>
     <t>级别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -360,7 +360,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -370,6 +370,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -454,15 +460,21 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,14 +484,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,7 +536,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -806,7 +824,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -814,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8280C78-A2C3-D342-A566-BA79FC172DBC}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -834,46 +852,52 @@
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:16" ht="26">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12">
+      <c r="C1" s="16">
+        <v>2023</v>
+      </c>
+      <c r="D1" s="17"/>
+      <c r="E1" s="14">
         <v>2022</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11">
+      <c r="F1" s="15"/>
+      <c r="G1" s="13">
         <v>2021</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13">
         <v>2020</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13">
         <v>2019</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13">
         <v>2018</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="2">
+      <c r="N1" s="13"/>
+      <c r="O1" s="2">
         <v>2017</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="31">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="8" t="s">
+    <row r="2" spans="1:16" ht="31">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="18" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
@@ -903,19 +927,25 @@
       <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="31">
+      <c r="N2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" ht="31">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="19">
         <v>31</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="4">
         <v>31</v>
       </c>
@@ -935,239 +965,279 @@
       <c r="M3" s="4">
         <v>31</v>
       </c>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="31">
+      <c r="N3" s="4"/>
+      <c r="O3" s="4">
+        <v>31</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" ht="31">
       <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4">
-        <v>342</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4" s="19">
+        <v>339</v>
+      </c>
+      <c r="D4" s="19">
         <f>C4-E4</f>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="E4" s="4">
         <v>342</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4">
+        <f>E4-G4</f>
+        <v>0</v>
+      </c>
       <c r="G4" s="4">
         <v>342</v>
       </c>
-      <c r="H4" s="4">
-        <f>G4-I4</f>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4">
+        <v>342</v>
+      </c>
+      <c r="J4" s="4">
+        <f>I4-K4</f>
         <v>-1</v>
       </c>
-      <c r="I4" s="4">
-        <v>343</v>
-      </c>
-      <c r="J4" s="4"/>
       <c r="K4" s="4">
         <v>343</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4">
+        <v>343</v>
+      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4">
         <v>344</v>
       </c>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="31">
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16" ht="31">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="19">
+        <v>3261</v>
+      </c>
+      <c r="D5" s="19">
+        <f t="shared" ref="D5:D8" si="0">C5-E5</f>
+        <v>-6</v>
+      </c>
+      <c r="E5" s="4">
         <v>3267</v>
       </c>
-      <c r="D5" s="4">
-        <f t="shared" ref="D5:D8" si="0">C5-E5</f>
+      <c r="F5" s="4">
+        <f t="shared" ref="F5:F8" si="1">E5-G5</f>
         <v>-4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="G5" s="4">
         <v>3271</v>
       </c>
-      <c r="F5" s="4">
-        <f>E5-G5</f>
+      <c r="H5" s="4">
+        <f>G5-I5</f>
         <v>-1</v>
       </c>
-      <c r="G5" s="4">
+      <c r="I5" s="4">
         <v>3272</v>
       </c>
-      <c r="H5" s="4">
-        <f t="shared" ref="H5:H8" si="1">G5-I5</f>
+      <c r="J5" s="4">
+        <f t="shared" ref="J5:J8" si="2">I5-K5</f>
         <v>-10</v>
       </c>
-      <c r="I5" s="4">
+      <c r="K5" s="4">
         <v>3282</v>
-      </c>
-      <c r="J5" s="4">
-        <f>I5-K5</f>
-        <v>-5</v>
-      </c>
-      <c r="K5" s="4">
-        <v>3287</v>
       </c>
       <c r="L5" s="4">
         <f>K5-M5</f>
+        <v>-5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>3287</v>
+      </c>
+      <c r="N5" s="4">
+        <f>M5-O5</f>
         <v>154</v>
       </c>
-      <c r="M5" s="4">
+      <c r="O5" s="4">
         <v>3133</v>
       </c>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="31">
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16" ht="31">
       <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="19">
+        <v>41350</v>
+      </c>
+      <c r="D6" s="19">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="E6" s="4">
         <v>41313</v>
       </c>
-      <c r="D6" s="4">
-        <f t="shared" si="0"/>
+      <c r="F6" s="4">
+        <f t="shared" si="1"/>
         <v>-300</v>
       </c>
-      <c r="E6" s="4">
+      <c r="G6" s="4">
         <v>41613</v>
       </c>
-      <c r="F6" s="4">
-        <f t="shared" ref="F6:F7" si="2">E6-G6</f>
+      <c r="H6" s="4">
+        <f t="shared" ref="H6:H7" si="3">G6-I6</f>
         <v>-1491</v>
       </c>
-      <c r="G6" s="4">
+      <c r="I6" s="4">
         <v>43104</v>
       </c>
-      <c r="H6" s="4">
-        <f t="shared" si="1"/>
+      <c r="J6" s="4">
+        <f t="shared" si="2"/>
         <v>-459</v>
       </c>
-      <c r="I6" s="4">
+      <c r="K6" s="4">
         <v>43563</v>
-      </c>
-      <c r="J6" s="4">
-        <f t="shared" ref="J6:J8" si="3">I6-K6</f>
-        <v>40</v>
-      </c>
-      <c r="K6" s="4">
-        <v>43523</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" ref="L6:L8" si="4">K6-M6</f>
+        <v>40</v>
+      </c>
+      <c r="M6" s="4">
+        <v>43523</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" ref="N6:N8" si="5">M6-O6</f>
         <v>655</v>
       </c>
-      <c r="M6" s="4">
+      <c r="O6" s="4">
         <v>42868</v>
       </c>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="31">
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16" ht="31">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="19">
+        <v>619502</v>
+      </c>
+      <c r="D7" s="19">
+        <f t="shared" si="0"/>
+        <v>9506</v>
+      </c>
+      <c r="E7" s="4">
         <v>609996</v>
       </c>
-      <c r="D7" s="4">
-        <f t="shared" si="0"/>
+      <c r="F7" s="4">
+        <f t="shared" si="1"/>
         <v>-23984</v>
       </c>
-      <c r="E7" s="4">
+      <c r="G7" s="4">
         <v>633980</v>
       </c>
-      <c r="F7" s="4">
+      <c r="H7" s="4">
+        <f t="shared" si="3"/>
+        <v>-24021</v>
+      </c>
+      <c r="I7" s="4">
+        <v>658001</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="2"/>
-        <v>-24021</v>
-      </c>
-      <c r="G7" s="4">
-        <v>658001</v>
-      </c>
-      <c r="H7" s="4">
-        <f t="shared" si="1"/>
         <v>-8259</v>
       </c>
-      <c r="I7" s="4">
+      <c r="K7" s="4">
         <v>666260</v>
-      </c>
-      <c r="J7" s="4">
-        <f t="shared" si="3"/>
-        <v>-7478</v>
-      </c>
-      <c r="K7" s="4">
-        <v>673738</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="4"/>
+        <v>-7478</v>
+      </c>
+      <c r="M7" s="4">
+        <v>673738</v>
+      </c>
+      <c r="N7" s="4">
+        <f t="shared" si="5"/>
         <v>7083</v>
       </c>
-      <c r="M7" s="4">
+      <c r="O7" s="4">
         <v>666655</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" ht="31">
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" ht="31">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="9">
+      <c r="C8" s="20">
         <f>SUM(C3:C7)</f>
+        <v>664483</v>
+      </c>
+      <c r="D8" s="20">
+        <f t="shared" si="0"/>
+        <v>9534</v>
+      </c>
+      <c r="E8" s="8">
+        <f>SUM(E3:E7)</f>
         <v>654949</v>
       </c>
-      <c r="D8" s="9">
-        <f t="shared" si="0"/>
+      <c r="F8" s="8">
+        <f t="shared" si="1"/>
         <v>-24288</v>
       </c>
-      <c r="E8" s="9">
-        <f>SUM(E3:E7)</f>
+      <c r="G8" s="8">
+        <f>SUM(G3:G7)</f>
         <v>679237</v>
       </c>
-      <c r="F8" s="9">
-        <f>SUM(F3:F7)</f>
+      <c r="H8" s="8">
+        <f>SUM(H3:H7)</f>
         <v>-25513</v>
       </c>
-      <c r="G8" s="6">
-        <f>SUM(G3:G7)</f>
+      <c r="I8" s="6">
+        <f>SUM(I3:I7)</f>
         <v>704750</v>
       </c>
-      <c r="H8" s="7">
-        <f t="shared" si="1"/>
+      <c r="J8" s="7">
+        <f t="shared" si="2"/>
         <v>-8729</v>
-      </c>
-      <c r="I8" s="5">
-        <f>SUM(I3:I7)</f>
-        <v>713479</v>
-      </c>
-      <c r="J8" s="5">
-        <f t="shared" si="3"/>
-        <v>-7443</v>
       </c>
       <c r="K8" s="5">
         <f>SUM(K3:K7)</f>
-        <v>720922</v>
+        <v>713479</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="4"/>
-        <v>7891</v>
+        <v>-7443</v>
       </c>
       <c r="M8" s="5">
         <f>SUM(M3:M7)</f>
+        <v>720922</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="5"/>
+        <v>7891</v>
+      </c>
+      <c r="O8" s="5">
+        <f>SUM(O3:O7)</f>
         <v>713031</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" ht="31">
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16" ht="31">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1182,8 +1252,10 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" ht="31">
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16" ht="31">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1198,8 +1270,10 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" ht="31">
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16" ht="31">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1214,8 +1288,10 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14" ht="31">
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16" ht="31">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1230,14 +1306,17 @@
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="C1:D1"/>
   </mergeCells>
@@ -1251,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79B5008C-D4E2-5C47-B9DB-CAF5560D9140}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1281,7 +1360,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
@@ -1297,11 +1376,11 @@
         <v>349</v>
       </c>
       <c r="F2">
-        <v>168</v>
+        <v>7470</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
@@ -1314,14 +1393,14 @@
         <v>16</v>
       </c>
       <c r="E3">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="F3">
-        <v>5573</v>
+        <v>5600</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="9" t="s">
         <v>48</v>
       </c>
       <c r="B4" t="s">
@@ -1334,14 +1413,14 @@
         <v>201</v>
       </c>
       <c r="E4">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="F4">
-        <v>53817</v>
+        <v>53976</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="9" t="s">
         <v>49</v>
       </c>
       <c r="B5" t="s">
@@ -1354,14 +1433,14 @@
         <v>133</v>
       </c>
       <c r="E5">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="F5">
-        <v>21865</v>
+        <v>21875</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="9" t="s">
         <v>50</v>
       </c>
       <c r="B6" t="s">
@@ -1374,14 +1453,14 @@
         <v>117</v>
       </c>
       <c r="E6">
-        <v>1228</v>
+        <v>1218</v>
       </c>
       <c r="F6">
-        <v>14467</v>
+        <v>14524</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="9" t="s">
         <v>51</v>
       </c>
       <c r="B7" t="s">
@@ -1394,14 +1473,14 @@
         <v>114</v>
       </c>
       <c r="E7">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="F7">
-        <v>16399</v>
+        <v>16513</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="9" t="s">
         <v>52</v>
       </c>
       <c r="B8" t="s">
@@ -1414,14 +1493,14 @@
         <v>77</v>
       </c>
       <c r="E8">
-        <v>1059</v>
+        <v>1063</v>
       </c>
       <c r="F8">
-        <v>11755</v>
+        <v>11812</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B9" t="s">
@@ -1434,14 +1513,14 @@
         <v>139</v>
       </c>
       <c r="E9">
-        <v>1728</v>
+        <v>1720</v>
       </c>
       <c r="F9">
-        <v>13919</v>
+        <v>13930</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B10" t="s">
@@ -1457,11 +1536,11 @@
         <v>234</v>
       </c>
       <c r="F10">
-        <v>6234</v>
+        <v>6396</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="9" t="s">
         <v>55</v>
       </c>
       <c r="B11" t="s">
@@ -1474,14 +1553,14 @@
         <v>119</v>
       </c>
       <c r="E11">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="F11">
-        <v>21946</v>
+        <v>21881</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="9" t="s">
         <v>56</v>
       </c>
       <c r="B12" t="s">
@@ -1491,17 +1570,17 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>1384</v>
       </c>
       <c r="F12">
-        <v>25306</v>
+        <v>25475</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B13" t="s">
@@ -1514,14 +1593,14 @@
         <v>135</v>
       </c>
       <c r="E13">
-        <v>1661</v>
+        <v>1682</v>
       </c>
       <c r="F13">
-        <v>18236</v>
+        <v>18283</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="9" t="s">
         <v>58</v>
       </c>
       <c r="B14" t="s">
@@ -1534,14 +1613,14 @@
         <v>93</v>
       </c>
       <c r="E14">
-        <v>1165</v>
+        <v>1170</v>
       </c>
       <c r="F14">
-        <v>17375</v>
+        <v>17441</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="9" t="s">
         <v>59</v>
       </c>
       <c r="B15" t="s">
@@ -1554,14 +1633,14 @@
         <v>111</v>
       </c>
       <c r="E15">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="F15">
-        <v>21778</v>
+        <v>21957</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="9" t="s">
         <v>60</v>
       </c>
       <c r="B16" t="s">
@@ -1571,17 +1650,17 @@
         <v>16</v>
       </c>
       <c r="D16">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E16">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="F16">
-        <v>62081</v>
+        <v>62079</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="9" t="s">
         <v>61</v>
       </c>
       <c r="B17" t="s">
@@ -1594,14 +1673,14 @@
         <v>198</v>
       </c>
       <c r="E17">
-        <v>2542</v>
+        <v>2585</v>
       </c>
       <c r="F17">
-        <v>51218</v>
+        <v>52348</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="9" t="s">
         <v>62</v>
       </c>
       <c r="B18" t="s">
@@ -1614,14 +1693,14 @@
         <v>117</v>
       </c>
       <c r="E18">
-        <v>1487</v>
+        <v>1475</v>
       </c>
       <c r="F18">
-        <v>27713</v>
+        <v>27397</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="9" t="s">
         <v>63</v>
       </c>
       <c r="B19" t="s">
@@ -1631,37 +1710,37 @@
         <v>14</v>
       </c>
       <c r="D19">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E19">
         <v>2008</v>
       </c>
       <c r="F19">
-        <v>29499</v>
+        <v>29521</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="9" t="s">
         <v>64</v>
       </c>
       <c r="B20" t="s">
         <v>34</v>
       </c>
       <c r="C20">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20">
         <v>141</v>
       </c>
       <c r="E20">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F20">
-        <v>26735</v>
+        <v>26797</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="9" t="s">
         <v>65</v>
       </c>
       <c r="B21" t="s">
@@ -1674,34 +1753,34 @@
         <v>125</v>
       </c>
       <c r="E21">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="F21">
-        <v>16610</v>
+        <v>16647</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22">
         <v>28</v>
       </c>
       <c r="E22">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F22">
-        <v>3294</v>
+        <v>3290</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B23" t="s">
@@ -1717,11 +1796,11 @@
         <v>1031</v>
       </c>
       <c r="F23">
-        <v>11234</v>
+        <v>11252</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B24" t="s">
@@ -1731,17 +1810,17 @@
         <v>21</v>
       </c>
       <c r="D24">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E24">
         <v>3111</v>
       </c>
       <c r="F24">
-        <v>34403</v>
+        <v>34394</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="9" t="s">
         <v>69</v>
       </c>
       <c r="B25" t="s">
@@ -1754,14 +1833,14 @@
         <v>93</v>
       </c>
       <c r="E25">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="F25">
-        <v>17920</v>
+        <v>17936</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="9" t="s">
         <v>70</v>
       </c>
       <c r="B26" t="s">
@@ -1774,14 +1853,14 @@
         <v>137</v>
       </c>
       <c r="E26">
-        <v>1458</v>
+        <v>1464</v>
       </c>
       <c r="F26">
-        <v>14771</v>
+        <v>14846</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B27" t="s">
@@ -1794,14 +1873,14 @@
         <v>80</v>
       </c>
       <c r="E27">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="F27">
-        <v>5557</v>
+        <v>5570</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="9" t="s">
         <v>72</v>
       </c>
       <c r="B28" t="s">
@@ -1817,11 +1896,11 @@
         <v>1336</v>
       </c>
       <c r="F28">
-        <v>20154</v>
+        <v>20270</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B29" t="s">
@@ -1834,14 +1913,14 @@
         <v>99</v>
       </c>
       <c r="E29">
-        <v>1405</v>
+        <v>1403</v>
       </c>
       <c r="F29">
-        <v>17614</v>
+        <v>17684</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="9" t="s">
         <v>74</v>
       </c>
       <c r="B30" t="s">
@@ -1857,11 +1936,11 @@
         <v>422</v>
       </c>
       <c r="F30">
-        <v>4717</v>
+        <v>4715</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="9" t="s">
         <v>75</v>
       </c>
       <c r="B31" t="s">
@@ -1874,14 +1953,14 @@
         <v>27</v>
       </c>
       <c r="E31">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F31">
-        <v>2900</v>
+        <v>2909</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="9" t="s">
         <v>76</v>
       </c>
       <c r="B32" t="s">
@@ -1894,35 +1973,35 @@
         <v>110</v>
       </c>
       <c r="E32">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="F32">
-        <v>14738</v>
+        <v>14714</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="11">
         <f>SUM(C33:F33)+31</f>
-        <v>654949</v>
-      </c>
-      <c r="C33" s="16">
+        <v>664483</v>
+      </c>
+      <c r="C33" s="11">
         <f>SUM(C2:C32)</f>
-        <v>342</v>
-      </c>
-      <c r="D33" s="16">
+        <v>339</v>
+      </c>
+      <c r="D33" s="11">
         <f>SUM(D2:D32)</f>
-        <v>3267</v>
-      </c>
-      <c r="E33" s="16">
+        <v>3261</v>
+      </c>
+      <c r="E33" s="11">
         <f>SUM(E2:E32)</f>
-        <v>41313</v>
-      </c>
-      <c r="F33" s="16">
+        <v>41350</v>
+      </c>
+      <c r="F33" s="11">
         <f>SUM(F2:F32)</f>
-        <v>609996</v>
+        <v>619502</v>
       </c>
     </row>
   </sheetData>

</xml_diff>